<commit_message>
add response to reviewers
</commit_message>
<xml_diff>
--- a/Paper Draft/response to reviewers/summary_per_strain.xlsx
+++ b/Paper Draft/response to reviewers/summary_per_strain.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanju\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\lung_particle_deposition_analysis\Paper Draft\response to reviewers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B0E835-CD5A-414B-912E-6584BE08B795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8A3539-BEB9-4ACE-BE18-851EB25FF738}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>Standard Deviations</t>
+  </si>
+  <si>
+    <t>table of measured values during/post aerosol exposure (summary per strain)</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -318,9 +324,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,230 +613,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6D8B33-1EC4-4C3F-9663-56E7032CC5DE}">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" t="s">
         <v>56</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1105</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>189</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.22</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.95</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" t="s">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>39</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>26</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.03</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.11</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
         <v>56</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1131</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>223</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.23</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.78</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>41</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>23</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.04</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.11</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1156</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>233</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.24</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.81</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>124</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>25</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.03</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.12</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1196</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>163</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.3</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.8</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>48</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.04</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.1</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -837,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ34"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,23 +996,23 @@
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1">
-        <f>C2</f>
+        <f t="shared" ref="O2:O34" si="0">C2</f>
         <v>1154.3499999999999</v>
       </c>
       <c r="P2" s="1">
-        <f>G2</f>
+        <f t="shared" ref="P2:P34" si="1">G2</f>
         <v>163.64999999999998</v>
       </c>
       <c r="Q2" s="1">
-        <f>I2</f>
+        <f t="shared" ref="Q2:Q34" si="2">I2</f>
         <v>0.21</v>
       </c>
       <c r="R2" s="1">
-        <f>M2</f>
+        <f t="shared" ref="R2:R34" si="3">M2</f>
         <v>0.83499999999999996</v>
       </c>
       <c r="S2" s="1">
-        <f>K2</f>
+        <f t="shared" ref="S2:S34" si="4">K2</f>
         <v>35.5</v>
       </c>
     </row>
@@ -1024,23 +1058,23 @@
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1">
-        <f>C3</f>
+        <f t="shared" si="0"/>
         <v>1067.1400000000001</v>
       </c>
       <c r="P3" s="1">
-        <f>G3</f>
+        <f t="shared" si="1"/>
         <v>149.30000000000001</v>
       </c>
       <c r="Q3" s="1">
-        <f>I3</f>
+        <f t="shared" si="2"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="R3" s="1">
-        <f>M3</f>
+        <f t="shared" si="3"/>
         <v>1.0649999999999999</v>
       </c>
       <c r="S3" s="1">
-        <f>K3</f>
+        <f t="shared" si="4"/>
         <v>24.2</v>
       </c>
     </row>
@@ -1086,23 +1120,23 @@
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1">
-        <f>C4</f>
+        <f t="shared" si="0"/>
         <v>1103.3499999999999</v>
       </c>
       <c r="P4" s="1">
-        <f>G4</f>
+        <f t="shared" si="1"/>
         <v>168.39999999999998</v>
       </c>
       <c r="Q4" s="1">
-        <f>I4</f>
+        <f t="shared" si="2"/>
         <v>0.215</v>
       </c>
       <c r="R4" s="1">
-        <f>M4</f>
+        <f t="shared" si="3"/>
         <v>0.95</v>
       </c>
       <c r="S4" s="1">
-        <f>K4</f>
+        <f t="shared" si="4"/>
         <v>40.5</v>
       </c>
     </row>
@@ -1148,23 +1182,23 @@
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>1097.3</v>
       </c>
       <c r="P5" s="1">
-        <f>G5</f>
+        <f t="shared" si="1"/>
         <v>217.3</v>
       </c>
       <c r="Q5" s="1">
-        <f>I5</f>
+        <f t="shared" si="2"/>
         <v>0.20499999999999999</v>
       </c>
       <c r="R5" s="1">
-        <f>M5</f>
+        <f t="shared" si="3"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="S5" s="1">
-        <f>K5</f>
+        <f t="shared" si="4"/>
         <v>47.85</v>
       </c>
     </row>
@@ -1210,23 +1244,23 @@
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>1075.8399999999999</v>
       </c>
       <c r="P6" s="1">
-        <f>G6</f>
+        <f t="shared" si="1"/>
         <v>186.45</v>
       </c>
       <c r="Q6" s="1">
-        <f>I6</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="R6" s="1">
-        <f>M6</f>
+        <f t="shared" si="3"/>
         <v>0.83499999999999996</v>
       </c>
       <c r="S6" s="1">
-        <f>K6</f>
+        <f t="shared" si="4"/>
         <v>47.3</v>
       </c>
     </row>
@@ -1272,23 +1306,23 @@
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>1078.04</v>
       </c>
       <c r="P7" s="1">
-        <f>G7</f>
+        <f t="shared" si="1"/>
         <v>204.1</v>
       </c>
       <c r="Q7" s="1" t="str">
-        <f>I7</f>
+        <f t="shared" si="2"/>
         <v>NA</v>
       </c>
       <c r="R7" s="1" t="str">
-        <f>M7</f>
+        <f t="shared" si="3"/>
         <v>NA</v>
       </c>
       <c r="S7" s="1" t="str">
-        <f>K7</f>
+        <f t="shared" si="4"/>
         <v>NA</v>
       </c>
       <c r="U7" t="s">
@@ -1340,23 +1374,23 @@
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1">
-        <f>C8</f>
+        <f t="shared" si="0"/>
         <v>1085.74</v>
       </c>
       <c r="P8" s="1">
-        <f>G8</f>
+        <f t="shared" si="1"/>
         <v>200.05</v>
       </c>
       <c r="Q8" s="1">
-        <f>I8</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="R8" s="1">
-        <f>M8</f>
+        <f t="shared" si="3"/>
         <v>0.92</v>
       </c>
       <c r="S8" s="1">
-        <f>K8</f>
+        <f t="shared" si="4"/>
         <v>39.799999999999997</v>
       </c>
       <c r="AQ8" s="1"/>
@@ -1403,23 +1437,23 @@
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>1175.21</v>
       </c>
       <c r="P9" s="1">
-        <f>G9</f>
+        <f t="shared" si="1"/>
         <v>221.65</v>
       </c>
       <c r="Q9" s="1">
-        <f>I9</f>
+        <f t="shared" si="2"/>
         <v>0.26500000000000001</v>
       </c>
       <c r="R9" s="1">
-        <f>M9</f>
+        <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
       <c r="S9" s="1">
-        <f>K9</f>
+        <f t="shared" si="4"/>
         <v>58.45</v>
       </c>
       <c r="U9">
@@ -1427,19 +1461,19 @@
         <v>1104.6212499999999</v>
       </c>
       <c r="V9">
-        <f t="shared" ref="V9:Y9" si="0">AVERAGE(P2:P9)</f>
+        <f t="shared" ref="V9:Y9" si="5">AVERAGE(P2:P9)</f>
         <v>188.86249999999998</v>
       </c>
       <c r="W9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.21571428571428569</v>
       </c>
       <c r="X9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.95071428571428562</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>41.942857142857143</v>
       </c>
       <c r="AA9">
@@ -1447,19 +1481,19 @@
         <v>39.292321837187764</v>
       </c>
       <c r="AB9">
-        <f t="shared" ref="AB9:AE9" si="1">STDEV(P2:P9)</f>
+        <f t="shared" ref="AB9:AE9" si="6">STDEV(P2:P9)</f>
         <v>26.366777662158867</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>3.3094381626464837E-2</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.11421575239536057</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10.794073550311003</v>
       </c>
     </row>
@@ -1504,23 +1538,23 @@
         <v>0.81499999999999995</v>
       </c>
       <c r="O10">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>1142.07</v>
       </c>
       <c r="P10">
-        <f>G10</f>
+        <f t="shared" si="1"/>
         <v>241.2</v>
       </c>
       <c r="Q10">
-        <f>I10</f>
+        <f t="shared" si="2"/>
         <v>0.155</v>
       </c>
       <c r="R10">
-        <f>M10</f>
+        <f t="shared" si="3"/>
         <v>0.81499999999999995</v>
       </c>
       <c r="S10">
-        <f>K10</f>
+        <f t="shared" si="4"/>
         <v>39.75</v>
       </c>
       <c r="AQ10" s="1"/>
@@ -1566,23 +1600,23 @@
         <v>0.77500000000000002</v>
       </c>
       <c r="O11">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>1128.4000000000001</v>
       </c>
       <c r="P11">
-        <f>G11</f>
+        <f t="shared" si="1"/>
         <v>225.25</v>
       </c>
       <c r="Q11">
-        <f>I11</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="R11">
-        <f>M11</f>
+        <f t="shared" si="3"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="S11">
-        <f>K11</f>
+        <f t="shared" si="4"/>
         <v>57.05</v>
       </c>
     </row>
@@ -1627,23 +1661,23 @@
         <v>0.73499999999999999</v>
       </c>
       <c r="O12">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>1144.6600000000001</v>
       </c>
       <c r="P12">
-        <f>G12</f>
+        <f t="shared" si="1"/>
         <v>229.3</v>
       </c>
       <c r="Q12">
-        <f>I12</f>
+        <f t="shared" si="2"/>
         <v>0.20499999999999999</v>
       </c>
       <c r="R12">
-        <f>M12</f>
+        <f t="shared" si="3"/>
         <v>0.73499999999999999</v>
       </c>
       <c r="S12">
-        <f>K12</f>
+        <f t="shared" si="4"/>
         <v>46.75</v>
       </c>
     </row>
@@ -1688,23 +1722,23 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="O13">
-        <f>C13</f>
+        <f t="shared" si="0"/>
         <v>1166.22</v>
       </c>
       <c r="P13">
-        <f>G13</f>
+        <f t="shared" si="1"/>
         <v>215.9</v>
       </c>
       <c r="Q13">
-        <f>I13</f>
+        <f t="shared" si="2"/>
         <v>0.215</v>
       </c>
       <c r="R13">
-        <f>M13</f>
+        <f t="shared" si="3"/>
         <v>0.92500000000000004</v>
       </c>
       <c r="S13">
-        <f>K13</f>
+        <f t="shared" si="4"/>
         <v>46.85</v>
       </c>
     </row>
@@ -1749,23 +1783,23 @@
         <v>0.85</v>
       </c>
       <c r="O14">
-        <f>C14</f>
+        <f t="shared" si="0"/>
         <v>1123.0899999999999</v>
       </c>
       <c r="P14">
-        <f>G14</f>
+        <f t="shared" si="1"/>
         <v>234.14999999999998</v>
       </c>
       <c r="Q14">
-        <f>I14</f>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="R14">
-        <f>M14</f>
+        <f t="shared" si="3"/>
         <v>0.85</v>
       </c>
       <c r="S14">
-        <f>K14</f>
+        <f t="shared" si="4"/>
         <v>64.5</v>
       </c>
     </row>
@@ -1810,23 +1844,23 @@
         <v>0.83499999999999996</v>
       </c>
       <c r="O15">
-        <f>C15</f>
+        <f t="shared" si="0"/>
         <v>1120.26</v>
       </c>
       <c r="P15">
-        <f>G15</f>
+        <f t="shared" si="1"/>
         <v>229.05</v>
       </c>
       <c r="Q15">
-        <f>I15</f>
+        <f t="shared" si="2"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="R15">
-        <f>M15</f>
+        <f t="shared" si="3"/>
         <v>0.83499999999999996</v>
       </c>
       <c r="S15">
-        <f>K15</f>
+        <f t="shared" si="4"/>
         <v>63.7</v>
       </c>
     </row>
@@ -1871,23 +1905,23 @@
         <v>0.83499999999999996</v>
       </c>
       <c r="O16">
-        <f>C16</f>
+        <f t="shared" si="0"/>
         <v>1163.07</v>
       </c>
       <c r="P16">
-        <f>G16</f>
+        <f t="shared" si="1"/>
         <v>246.2</v>
       </c>
       <c r="Q16">
-        <f>I16</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="R16">
-        <f>M16</f>
+        <f t="shared" si="3"/>
         <v>0.83499999999999996</v>
       </c>
       <c r="S16">
-        <f>K16</f>
+        <f t="shared" si="4"/>
         <v>62.15</v>
       </c>
     </row>
@@ -1932,23 +1966,23 @@
         <v>0.85499999999999998</v>
       </c>
       <c r="O17">
-        <f>C17</f>
+        <f t="shared" si="0"/>
         <v>1100.77</v>
       </c>
       <c r="P17">
-        <f>G17</f>
+        <f t="shared" si="1"/>
         <v>238.05</v>
       </c>
       <c r="Q17">
-        <f>I17</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="R17">
-        <f>M17</f>
+        <f t="shared" si="3"/>
         <v>0.85499999999999998</v>
       </c>
       <c r="S17">
-        <f>K17</f>
+        <f t="shared" si="4"/>
         <v>47.6</v>
       </c>
     </row>
@@ -1993,23 +2027,23 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="O18">
-        <f>C18</f>
+        <f t="shared" si="0"/>
         <v>1040.31</v>
       </c>
       <c r="P18">
-        <f>G18</f>
+        <f t="shared" si="1"/>
         <v>208.55</v>
       </c>
       <c r="Q18">
-        <f>I18</f>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="R18">
-        <f>M18</f>
+        <f t="shared" si="3"/>
         <v>0.70499999999999996</v>
       </c>
       <c r="S18">
-        <f>K18</f>
+        <f t="shared" si="4"/>
         <v>41.7</v>
       </c>
     </row>
@@ -2054,23 +2088,23 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="O19">
-        <f>C19</f>
+        <f t="shared" si="0"/>
         <v>1185.52</v>
       </c>
       <c r="P19">
-        <f>G19</f>
+        <f t="shared" si="1"/>
         <v>165.75</v>
       </c>
       <c r="Q19">
-        <f>I19</f>
+        <f t="shared" si="2"/>
         <v>0.23499999999999999</v>
       </c>
       <c r="R19">
-        <f>M19</f>
+        <f t="shared" si="3"/>
         <v>0.51500000000000001</v>
       </c>
       <c r="S19">
-        <f>K19</f>
+        <f t="shared" si="4"/>
         <v>38.700000000000003</v>
       </c>
       <c r="U19">
@@ -2156,23 +2190,23 @@
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1">
-        <f>C20</f>
+        <f t="shared" si="0"/>
         <v>1116.76</v>
       </c>
       <c r="P20" s="1">
-        <f>G20</f>
+        <f t="shared" si="1"/>
         <v>221.75</v>
       </c>
       <c r="Q20" s="1">
-        <f>I20</f>
+        <f t="shared" si="2"/>
         <v>0.22500000000000001</v>
       </c>
       <c r="R20" s="1">
-        <f>M20</f>
+        <f t="shared" si="3"/>
         <v>0.72</v>
       </c>
       <c r="S20" s="1">
-        <f>K20</f>
+        <f t="shared" si="4"/>
         <v>49.95</v>
       </c>
     </row>
@@ -2218,23 +2252,23 @@
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1">
-        <f>C21</f>
+        <f t="shared" si="0"/>
         <v>1055.43</v>
       </c>
       <c r="P21" s="1">
-        <f>G21</f>
+        <f t="shared" si="1"/>
         <v>194.3</v>
       </c>
       <c r="Q21" s="1">
-        <f>I21</f>
+        <f t="shared" si="2"/>
         <v>0.255</v>
       </c>
       <c r="R21" s="1">
-        <f>M21</f>
+        <f t="shared" si="3"/>
         <v>0.63500000000000001</v>
       </c>
       <c r="S21" s="1">
-        <f>K21</f>
+        <f t="shared" si="4"/>
         <v>49.15</v>
       </c>
     </row>
@@ -2280,23 +2314,23 @@
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1">
-        <f>C22</f>
+        <f t="shared" si="0"/>
         <v>1444.02</v>
       </c>
       <c r="P22" s="1">
-        <f>G22</f>
+        <f t="shared" si="1"/>
         <v>234.3</v>
       </c>
       <c r="Q22" s="1">
-        <f>I22</f>
+        <f t="shared" si="2"/>
         <v>0.26</v>
       </c>
       <c r="R22" s="1">
-        <f>M22</f>
+        <f t="shared" si="3"/>
         <v>0.81499999999999995</v>
       </c>
       <c r="S22" s="1">
-        <f>K22</f>
+        <f t="shared" si="4"/>
         <v>63.05</v>
       </c>
     </row>
@@ -2342,23 +2376,23 @@
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1">
-        <f>C23</f>
+        <f t="shared" si="0"/>
         <v>1122.8399999999999</v>
       </c>
       <c r="P23" s="1">
-        <f>G23</f>
+        <f t="shared" si="1"/>
         <v>275.64999999999998</v>
       </c>
       <c r="Q23" s="1">
-        <f>I23</f>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
       <c r="R23" s="1">
-        <f>M23</f>
+        <f t="shared" si="3"/>
         <v>0.79</v>
       </c>
       <c r="S23" s="1">
-        <f>K23</f>
+        <f t="shared" si="4"/>
         <v>66.55</v>
       </c>
     </row>
@@ -2404,23 +2438,23 @@
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1">
-        <f>C24</f>
+        <f t="shared" si="0"/>
         <v>1062.17</v>
       </c>
       <c r="P24" s="1">
-        <f>G24</f>
+        <f t="shared" si="1"/>
         <v>218.05</v>
       </c>
       <c r="Q24" s="1">
-        <f>I24</f>
+        <f t="shared" si="2"/>
         <v>0.19500000000000001</v>
       </c>
       <c r="R24" s="1">
-        <f>M24</f>
+        <f t="shared" si="3"/>
         <v>0.90500000000000003</v>
       </c>
       <c r="S24" s="1">
-        <f>K24</f>
+        <f t="shared" si="4"/>
         <v>42.55</v>
       </c>
     </row>
@@ -2466,23 +2500,23 @@
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1">
-        <f>C25</f>
+        <f t="shared" si="0"/>
         <v>1140.6500000000001</v>
       </c>
       <c r="P25" s="1">
-        <f>G25</f>
+        <f t="shared" si="1"/>
         <v>248.6</v>
       </c>
       <c r="Q25" s="1">
-        <f>I25</f>
+        <f t="shared" si="2"/>
         <v>0.27</v>
       </c>
       <c r="R25" s="1">
-        <f>M25</f>
+        <f t="shared" si="3"/>
         <v>0.72499999999999998</v>
       </c>
       <c r="S25" s="1">
-        <f>K25</f>
+        <f t="shared" si="4"/>
         <v>66.7</v>
       </c>
     </row>
@@ -2528,23 +2562,23 @@
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1">
-        <f>C26</f>
+        <f t="shared" si="0"/>
         <v>1186.47</v>
       </c>
       <c r="P26" s="1">
-        <f>G26</f>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="Q26" s="1">
-        <f>I26</f>
+        <f t="shared" si="2"/>
         <v>0.23</v>
       </c>
       <c r="R26" s="1">
-        <f>M26</f>
+        <f t="shared" si="3"/>
         <v>1.01</v>
       </c>
       <c r="S26" s="1">
-        <f>K26</f>
+        <f t="shared" si="4"/>
         <v>50.6</v>
       </c>
     </row>
@@ -2590,23 +2624,23 @@
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1">
-        <f>C27</f>
+        <f t="shared" si="0"/>
         <v>1118.92</v>
       </c>
       <c r="P27" s="1">
-        <f>G27</f>
+        <f t="shared" si="1"/>
         <v>250.89999999999998</v>
       </c>
       <c r="Q27" s="1">
-        <f>I27</f>
+        <f t="shared" si="2"/>
         <v>0.215</v>
       </c>
       <c r="R27" s="1">
-        <f>M27</f>
+        <f t="shared" si="3"/>
         <v>0.86</v>
       </c>
       <c r="S27" s="1">
-        <f>K27</f>
+        <f t="shared" si="4"/>
         <v>54.05</v>
       </c>
       <c r="U27">
@@ -2614,19 +2648,19 @@
         <v>1155.9075000000003</v>
       </c>
       <c r="V27">
-        <f t="shared" ref="V27:Y27" si="2">AVERAGE(P20:P27)</f>
+        <f t="shared" ref="V27:Y27" si="7">AVERAGE(P20:P27)</f>
         <v>232.94374999999997</v>
       </c>
       <c r="W27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.23625000000000002</v>
       </c>
       <c r="X27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.8075</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>55.325000000000003</v>
       </c>
       <c r="AA27">
@@ -2634,19 +2668,19 @@
         <v>123.66555055009108</v>
       </c>
       <c r="AB27">
-        <f t="shared" ref="AB27:AE27" si="3">STDEV(P20:P27)</f>
+        <f t="shared" ref="AB27:AE27" si="8">STDEV(P20:P27)</f>
         <v>25.074780122950362</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>2.5035688811888408E-2</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.11823100874377863</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>9.0177602540764106</v>
       </c>
     </row>
@@ -2691,23 +2725,23 @@
         <v>0.81</v>
       </c>
       <c r="O28">
-        <f>C28</f>
+        <f t="shared" si="0"/>
         <v>1224.19</v>
       </c>
       <c r="P28">
-        <f>G28</f>
+        <f t="shared" si="1"/>
         <v>97.6</v>
       </c>
       <c r="Q28">
-        <f>I28</f>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="R28">
-        <f>M28</f>
+        <f t="shared" si="3"/>
         <v>0.81</v>
       </c>
       <c r="S28">
-        <f>K28</f>
+        <f t="shared" si="4"/>
         <v>29.6</v>
       </c>
     </row>
@@ -2752,23 +2786,23 @@
         <v>0.69499999999999995</v>
       </c>
       <c r="O29">
-        <f>C29</f>
+        <f t="shared" si="0"/>
         <v>1211.21</v>
       </c>
       <c r="P29">
-        <f>G29</f>
+        <f t="shared" si="1"/>
         <v>129.94999999999999</v>
       </c>
       <c r="Q29">
-        <f>I29</f>
+        <f t="shared" si="2"/>
         <v>0.29499999999999998</v>
       </c>
       <c r="R29">
-        <f>M29</f>
+        <f t="shared" si="3"/>
         <v>0.69499999999999995</v>
       </c>
       <c r="S29">
-        <f>K29</f>
+        <f t="shared" si="4"/>
         <v>35.75</v>
       </c>
     </row>
@@ -2813,23 +2847,23 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="O30">
-        <f>C30</f>
+        <f t="shared" si="0"/>
         <v>1197.04</v>
       </c>
       <c r="P30">
-        <f>G30</f>
+        <f t="shared" si="1"/>
         <v>215.2</v>
       </c>
       <c r="Q30">
-        <f>I30</f>
+        <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
       <c r="R30">
-        <f>M30</f>
+        <f t="shared" si="3"/>
         <v>0.92500000000000004</v>
       </c>
       <c r="S30">
-        <f>K30</f>
+        <f t="shared" si="4"/>
         <v>77.95</v>
       </c>
     </row>
@@ -2874,23 +2908,23 @@
         <v>0.67</v>
       </c>
       <c r="O31">
-        <f>C31</f>
+        <f t="shared" si="0"/>
         <v>1202.26</v>
       </c>
       <c r="P31">
-        <f>G31</f>
+        <f t="shared" si="1"/>
         <v>117.05000000000001</v>
       </c>
       <c r="Q31">
-        <f>I31</f>
+        <f t="shared" si="2"/>
         <v>0.29499999999999998</v>
       </c>
       <c r="R31">
-        <f>M31</f>
+        <f t="shared" si="3"/>
         <v>0.67</v>
       </c>
       <c r="S31">
-        <f>K31</f>
+        <f t="shared" si="4"/>
         <v>46.6</v>
       </c>
     </row>
@@ -2935,23 +2969,23 @@
         <v>0.91</v>
       </c>
       <c r="O32">
-        <f>C32</f>
+        <f t="shared" si="0"/>
         <v>1143.7</v>
       </c>
       <c r="P32">
-        <f>G32</f>
+        <f t="shared" si="1"/>
         <v>200.05</v>
       </c>
       <c r="Q32">
-        <f>I32</f>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
       <c r="R32">
-        <f>M32</f>
+        <f t="shared" si="3"/>
         <v>0.91</v>
       </c>
       <c r="S32">
-        <f>K32</f>
+        <f t="shared" si="4"/>
         <v>48.15</v>
       </c>
     </row>
@@ -2996,23 +3030,23 @@
         <v>0.75</v>
       </c>
       <c r="O33">
-        <f>C33</f>
+        <f t="shared" si="0"/>
         <v>1224.76</v>
       </c>
       <c r="P33">
-        <f>G33</f>
+        <f t="shared" si="1"/>
         <v>170.2</v>
       </c>
       <c r="Q33">
-        <f>I33</f>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="R33">
-        <f>M33</f>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
       <c r="S33">
-        <f>K33</f>
+        <f t="shared" si="4"/>
         <v>52.25</v>
       </c>
     </row>
@@ -3057,23 +3091,23 @@
         <v>0.81499999999999995</v>
       </c>
       <c r="O34">
-        <f>C34</f>
+        <f t="shared" si="0"/>
         <v>1165.83</v>
       </c>
       <c r="P34">
-        <f>G34</f>
+        <f t="shared" si="1"/>
         <v>208.2</v>
       </c>
       <c r="Q34">
-        <f>I34</f>
+        <f t="shared" si="2"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="R34">
-        <f>M34</f>
+        <f t="shared" si="3"/>
         <v>0.81499999999999995</v>
       </c>
       <c r="S34">
-        <f>K34</f>
+        <f t="shared" si="4"/>
         <v>57.6</v>
       </c>
       <c r="U34">
@@ -3081,19 +3115,19 @@
         <v>1195.57</v>
       </c>
       <c r="V34">
-        <f t="shared" ref="V34:Y34" si="4">AVERAGE(P28:P34)</f>
+        <f t="shared" ref="V34:Y34" si="9">AVERAGE(P28:P34)</f>
         <v>162.60714285714286</v>
       </c>
       <c r="W34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.29499999999999998</v>
       </c>
       <c r="X34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.79642857142857137</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>49.7</v>
       </c>
       <c r="AA34">
@@ -3101,19 +3135,19 @@
         <v>30.379959403088971</v>
       </c>
       <c r="AB34">
-        <f t="shared" ref="AB34:AE34" si="5">STDEV(P28:P34)</f>
+        <f t="shared" ref="AB34:AE34" si="10">STDEV(P28:P34)</f>
         <v>47.735743321710039</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.5823642100341224E-2</v>
       </c>
       <c r="AD34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>9.8645589769399022E-2</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>15.692885861646539</v>
       </c>
     </row>
@@ -3131,7 +3165,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>